<commit_message>
Draup-Automation FW update-SignIN,Universe-Done Required Changes-Renuka-10-11-17.
</commit_message>
<xml_diff>
--- a/TestData/Locators.xlsx
+++ b/TestData/Locators.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="31" documentId="C4CCDBD366EDBDE275BBD94F672EBC5E114D0565" xr6:coauthVersionLast="24" xr6:coauthVersionMax="24" xr10:uidLastSave="{E0FAC324-8A33-4433-9955-F4A482C1966C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="16365" windowHeight="6960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="16365" windowHeight="6960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Elements" sheetId="1" r:id="rId1"/>
-    <sheet name="LoginData" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="LoginData" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
   <si>
     <t>VariableName</t>
   </si>
@@ -63,9 +63,6 @@
     <t>ClickOnContender</t>
   </si>
   <si>
-    <t>Universe</t>
-  </si>
-  <si>
     <t>ClickOnUniverseLink</t>
   </si>
   <si>
@@ -73,13 +70,97 @@
   </si>
   <si>
     <t>//*[@id='root']//a[.='Contenders']</t>
+  </si>
+  <si>
+    <t>//div[@class='text-left ag-header-cell-label'][@title='Account']</t>
+  </si>
+  <si>
+    <t>TableAccoutHeader</t>
+  </si>
+  <si>
+    <t>//div[@class='text-center ag-header-cell-label'][@title='Opportunity Index']</t>
+  </si>
+  <si>
+    <t>automotive</t>
+  </si>
+  <si>
+    <t>//label[text()='Automotive']</t>
+  </si>
+  <si>
+    <t>consumersoftware</t>
+  </si>
+  <si>
+    <t>//label[text()='Consumer Software']</t>
+  </si>
+  <si>
+    <t>enterprisesoftware</t>
+  </si>
+  <si>
+    <t>//label[text()='Enterprise Software']</t>
+  </si>
+  <si>
+    <t>//h6[text()='Subverticals']</t>
+  </si>
+  <si>
+    <t>//div[@class='text-center ag-header-cell-label'][@title='Base Opportunity Index']</t>
+  </si>
+  <si>
+    <t>Universe,Opportunity</t>
+  </si>
+  <si>
+    <t>TableOpportunityIndex</t>
+  </si>
+  <si>
+    <t>BaseOpportunityIndex</t>
+  </si>
+  <si>
+    <t>IncrementalOpportunity</t>
+  </si>
+  <si>
+    <t>HiringSignal</t>
+  </si>
+  <si>
+    <t>InvestementSignals</t>
+  </si>
+  <si>
+    <t>M&amp;Asignal</t>
+  </si>
+  <si>
+    <t>LayoffSignal</t>
+  </si>
+  <si>
+    <t>ExecutiveMovement</t>
+  </si>
+  <si>
+    <t>//div[@class='text-center ag-header-cell-label'][@title='Incremental Opportunity Index']</t>
+  </si>
+  <si>
+    <t>//div[@class='text-center ag-header-cell-label'][@title='Hiring Signal']</t>
+  </si>
+  <si>
+    <t>//div[@class='text-center ag-header-cell-label'][@title='Investments Signal']</t>
+  </si>
+  <si>
+    <t>//div[@class='text-center ag-header-cell-label'][@title='M&amp;A Signal']</t>
+  </si>
+  <si>
+    <t>//div[@class='text-center ag-header-cell-label'][@title='Layoff/Attrition Signal']</t>
+  </si>
+  <si>
+    <t>subverticals</t>
+  </si>
+  <si>
+    <t>//div[@class='text-center ag-header-cell-label'][@title='Executive Movement Signal']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  UN=new UniversePageObjects(driver, test)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,6 +175,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -143,12 +230,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,18 +605,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="27.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="55.7109375" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="2"/>
+    <col min="3" max="3" width="81.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -581,54 +672,170 @@
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+      <c r="A8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="A9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
+      <c r="A10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
+      <c r="A11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
+      <c r="A12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
+      <c r="A13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -637,6 +844,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C976C5C8-ADC4-40F5-A201-C00B7BE53C8D}">
+  <dimension ref="E1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>

</xml_diff>

<commit_message>
Universe - Account commit-Renuka Sisodia-11/11/17
</commit_message>
<xml_diff>
--- a/TestData/Locators.xlsx
+++ b/TestData/Locators.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="16365" windowHeight="6960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="16365" windowHeight="6960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Elements" sheetId="1" r:id="rId1"/>
@@ -607,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -847,7 +847,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C976C5C8-ADC4-40F5-A201-C00B7BE53C8D}">
   <dimension ref="E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>

</xml_diff>